<commit_message>
Add deleting files from excel and picture view
</commit_message>
<xml_diff>
--- a/public/Goods.xlsx
+++ b/public/Goods.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jan PC\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Beibit\projects\satuline\saudaline-admin\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{058DEE94-CCFF-43A8-B630-EC84D1CC45D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E775C215-35F1-45BE-AA53-925D878D621F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F74236F7-6735-42F5-B181-FD8FE0854460}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F74236F7-6735-42F5-B181-FD8FE0854460}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="27">
   <si>
     <t>Тестовый продукт из EXCEL 2</t>
   </si>
@@ -109,23 +109,17 @@
   </si>
   <si>
     <t>Категория</t>
+  </si>
+  <si>
+    <t>Картинка товара</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -161,9 +155,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -179,6 +184,356 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>86611</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1171575</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Рисунок 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD0CD7D1-3237-9664-38EF-3F741F71D764}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="66675" y="277111"/>
+          <a:ext cx="1104900" cy="932564"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1181100</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>999239</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Рисунок 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1816635E-C442-42BB-A234-91828E830531}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="76200" y="1276350"/>
+          <a:ext cx="1104900" cy="932564"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>157544</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>86611</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1080705</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>1019175</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Рисунок 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F93C5DF5-CCD0-4AB5-89EF-7E5614B9CA18}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="157544" y="1296286"/>
+          <a:ext cx="923161" cy="932564"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>155931</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>86611</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1082319</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1019175</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Рисунок 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6DC0A606-6C86-42C3-8081-CC8DABA3F0AC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="155931" y="2334511"/>
+          <a:ext cx="926388" cy="932564"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>152843</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>86611</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1085407</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1019175</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Рисунок 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{721C7CA5-FC97-4C33-AB02-2DF52E898F76}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="152843" y="4544311"/>
+          <a:ext cx="932564" cy="932564"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>197607</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1171575</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>908178</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Рисунок 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4687F27D-DA46-4F79-96C2-E636490EAEA6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="66675" y="5741157"/>
+          <a:ext cx="1104900" cy="710571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>152843</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>86611</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1085407</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>1019175</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Рисунок 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F4389569-C575-44F3-9933-EF65B2C4DD94}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="152843" y="6773161"/>
+          <a:ext cx="932564" cy="932564"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -478,201 +833,207 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{769FE122-F55F-4411-83C8-85081A63EB26}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.44140625" customWidth="1"/>
-    <col min="2" max="2" width="39.44140625" customWidth="1"/>
-    <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="13.88671875" customWidth="1"/>
-    <col min="6" max="6" width="35.21875" customWidth="1"/>
-    <col min="7" max="7" width="12.21875" customWidth="1"/>
-    <col min="8" max="8" width="15.77734375" customWidth="1"/>
+    <col min="1" max="1" width="24.28515625" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" customWidth="1"/>
+    <col min="3" max="3" width="39.42578125" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" customWidth="1"/>
+    <col min="7" max="7" width="35.28515625" customWidth="1"/>
+    <col min="8" max="8" width="29.5703125" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
         <v>20</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>21</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>22</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>23</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>24</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>25</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:8" s="1" customFormat="1" ht="87" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D2">
+      <c r="E2" s="2">
         <v>450</v>
       </c>
-      <c r="E2">
+      <c r="F2" s="2">
         <v>10000</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:8" s="1" customFormat="1" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D3">
+      <c r="E3" s="2">
         <v>123</v>
       </c>
-      <c r="E3">
+      <c r="F3" s="2">
         <v>9500</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="4" spans="1:8" s="1" customFormat="1" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D4">
+      <c r="E4" s="2">
         <v>850</v>
       </c>
-      <c r="E4">
+      <c r="F4" s="2">
         <v>8500</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="5" spans="1:8" s="1" customFormat="1" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D5">
+      <c r="E5" s="2">
         <v>470</v>
       </c>
-      <c r="E5">
+      <c r="F5" s="2">
         <v>7800</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="6" spans="1:8" s="1" customFormat="1" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D6">
+      <c r="E6" s="2">
         <v>690</v>
       </c>
-      <c r="E6">
+      <c r="F6" s="2">
         <v>9800</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="7" spans="1:8" s="1" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D7">
+      <c r="E7" s="2">
         <v>750</v>
       </c>
-      <c r="E7">
+      <c r="F7" s="2">
         <v>10500</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="8" spans="1:8" s="1" customFormat="1" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D8">
+      <c r="E8" s="2">
         <v>950</v>
       </c>
-      <c r="E8">
+      <c r="F8" s="2">
         <v>9600</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" s="1" t="s">
         <v>19</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>